<commit_message>
Ajuste de nota na tabela do Excel
</commit_message>
<xml_diff>
--- a/INF_ALP_2025.xlsx
+++ b/INF_ALP_2025.xlsx
@@ -359,7 +359,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,415 +384,421 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>202411909648</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>202511602542</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>202511602545</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>202511603200</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>202511602497</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>202511602473</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>202511602524</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>10</v>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>202511602491</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>202511602441</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>202511602567</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>202511602557</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>202511602452</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>202511603204</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>202511603162</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>202511602437</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>202511602537</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>202511602501</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>202511603157</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>202511603167</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>202511602444</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>202511602349</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>202511602536</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>202511602440</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>202511602492</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>202511602456</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>202511603158</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>202511602455</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>202511602443</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>202511602464</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>202511602459</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>202511602519</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>10</v>
+      <c r="C32" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>202511602519</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>202511602569</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>202511602470</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>202511602510</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>202511602518</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>202511602530</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>202511602513</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adaptação para trabalhar com várias disciplinas
</commit_message>
<xml_diff>
--- a/INF_ALP_2025.xlsx
+++ b/INF_ALP_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Matricula</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t xml:space="preserve">Recuperação 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuperação 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação 03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuperação 03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação 04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuperação 04</t>
   </si>
   <si>
     <t xml:space="preserve">ALEXSANDRO SOUZA DA SILVA</t>
@@ -356,10 +374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,6 +385,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,425 +402,662 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>202411909648</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>202511602542</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>202511602545</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>202511603200</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>202511602497</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>202511602473</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>202511602524</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>202511602491</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>202511602441</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>202511602567</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>202511602557</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>202511602452</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>202511603204</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>202511603162</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>202511602437</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>202511602537</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>202511602501</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>202511603157</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>202511603167</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>202511602444</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>202511602349</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>202511602536</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>202511602440</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>202511602492</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>202511602456</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>202511603158</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>202511602455</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>202511602443</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>202511602464</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>202511602459</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>202511602519</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>202511602519</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>202511602569</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>202511602470</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>202511602510</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>202511602518</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>202511602530</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>202511602513</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>